<commit_message>
Implementation: Added batch registration mode
</commit_message>
<xml_diff>
--- a/frontend/public/templates/certificate-template.xlsx
+++ b/frontend/public/templates/certificate-template.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="28827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="27726"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kyeongha\GitHub\certmanager\frontend\public\templates\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\thdbs\certmanager\frontend\public\templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{927D9A0A-F926-4D32-8ADC-DA3A5C99B3D0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C5EB6F37-47C0-4F2E-A359-1FDEAF8F72F9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="8385" yWindow="3570" windowWidth="21600" windowHeight="11295" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="4140" yWindow="2895" windowWidth="21600" windowHeight="11295" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="21">
   <si>
     <t>발급번호</t>
   </si>
@@ -494,7 +494,7 @@
   <dimension ref="A1:K2"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="C1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="G8" sqref="G8"/>
+      <selection activeCell="I3" sqref="I3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -571,8 +571,8 @@
       <c r="H2" t="s">
         <v>12</v>
       </c>
-      <c r="I2" t="s">
-        <v>9</v>
+      <c r="I2">
+        <v>12345</v>
       </c>
       <c r="J2" t="s">
         <v>9</v>

</xml_diff>